<commit_message>
nová verze 2.0, možnosti mountění, oprava chyb
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -27,11 +27,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Consolas"/>
-      <charset val="238"/>
-      <family val="3"/>
-      <color rgb="FFD16969"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
       <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -51,17 +52,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -426,16 +427,11 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5145566</t>
+          <t>dsff</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -450,14 +446,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>fffffffffffffffffffffffffffffff</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dsff</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -468,23 +464,18 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>fffffffffffffffffffffffffffffff</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>514</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.100.241</t>
+          <t>192.168.14.241</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -521,50 +512,86 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22.140625" customWidth="1" min="2" max="2"/>
+    <col width="8.42578125" customWidth="1" min="2" max="2"/>
+    <col width="32" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>518</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>\\192.168.208.200\10_vision</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>jhv_vision</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>první sít, ixon</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>514-2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>192.168.14.245\Data</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>\\192.168.14.245\Data\Kamery</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
         <is>
           <t>Vision</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>*Jhv2708</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>poznamky</t>
-        </is>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>

</xml_diff>

<commit_message>
vylepsena sprava pripojovani k diskum, zobrazovani staticke adresy, bindovani
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -427,6 +427,7 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -453,7 +454,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>51452422</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -464,18 +465,23 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>aha</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>192.168.14.241</t>
+          <t>192.168.100.241</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -487,22 +493,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>51452422</t>
+          <t>514</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.100.241</t>
+          <t>192.168.14.241</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>aha</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
vertikalni sloupec s oblibenymi projekty funkcni
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6015" yWindow="1965" windowWidth="28800" windowHeight="15885" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7650" yWindow="1470" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
@@ -406,8 +406,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -418,7 +418,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>51455</t>
+          <t>hostivař</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -431,14 +431,15 @@
           <t>255.255.255.0</t>
         </is>
       </c>
+      <c r="D1" t="inlineStr"/>
       <c r="E1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dsff</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -451,13 +452,8 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>fffffffffffffffffffffffffffffff</t>
-        </is>
-      </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -482,13 +478,13 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>omeleta</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -508,12 +504,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>514</t>
+          <t>brambora</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>192.168.14.241</t>
+          <t>192.168.1.241</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -536,10 +532,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -550,7 +546,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>51452422</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -563,44 +559,8 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>aha</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>51455</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>192.168.1.241</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>192.168.100.241</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>255.255.255.0</t>
-        </is>
+      <c r="E1" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mnoho oprav, moznosti menit statusy oblibenosti v editaci a pri pridavani noveho projektu
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -431,7 +431,6 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr"/>
       <c r="E1" t="n">
         <v>0</v>
       </c>
@@ -439,7 +438,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>jojo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -459,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>51452422</t>
+          <t>5145242</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -504,20 +503,46 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>brambora</t>
+          <t>todleto no</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>192.168.000.999</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>joo
+§j</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>brambor</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>192.168.1.241</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -546,7 +571,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>jojo</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -589,59 +614,59 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>514-2</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>první sít, ixon</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>514-2</t>
+          <t>518</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>první sít, ixon</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
plne funkcni verze ip manager, prace na uvodni strance trimazkonu
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7650" yWindow="1470" windowWidth="28800" windowHeight="15345" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6015" yWindow="1965" windowWidth="28800" windowHeight="15885" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="ip_address_list" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="ip_adress_fav_list" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="disc_list" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="disk_list" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Settings" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
@@ -404,10 +404,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -432,7 +432,7 @@
         </is>
       </c>
       <c r="E1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -443,16 +443,70 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>192.168.000.j</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>kkgg</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bewolktEN</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>192.168.000.000</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>du hast einen problem</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>einkaufenfh</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>gggg</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -469,8 +523,8 @@
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -481,7 +535,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>regenschrim</t>
+          <t>bewolktEN</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -492,6 +546,11 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>du hast einen problem</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -512,7 +571,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -595,10 +654,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -625,18 +684,38 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ethernet,Ethernet1,Ethernet2,Ethernet3,Ethernet4,Ethernet5,Wi-Fi,</t>
+          <t>Ethernet,Ethernet 1,Ethernet 2,Ethernet 3,Ethernet 4,Ethernet 5,Wi-Fi,</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>okno oblibene =&gt; 1</t>
+          <t>spousteci okno: na oblibenych = 1</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>spousteci okno: zobrazeni disku = 1, normal = 0</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>zakladni velikost okna normal = 0, max = 1,min = 2</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verze 3.6 nova visualizace, format tlacitek, zjistovani offline statusu disku, uprava otevirani suboken
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -404,7 +404,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
@@ -418,17 +418,22 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>regenschrim</t>
+          <t>kartoffelnsalat</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>192.168.000.000</t>
+          <t>192.168.000.j</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
           <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>kkgg</t>
         </is>
       </c>
       <c r="E1" t="n">
@@ -438,12 +443,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>kartoffelnsalat</t>
+          <t>einkaufenfh</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>192.168.000.j</t>
+          <t>192.168.000.000</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -453,17 +458,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>kkgg</t>
+          <t>gggg</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>bewolktEN</t>
+          <t>regenschrim</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -476,19 +481,14 @@
           <t>255.255.255.0</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>du hast einen problem</t>
-        </is>
-      </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>einkaufenfh</t>
+          <t>bewolktt</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -503,11 +503,36 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>gggg</t>
+          <t>du hast einen problem</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>hggh</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">joo				</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -521,7 +546,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -535,7 +560,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>bewolktEN</t>
+          <t>einkaufenfh</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -550,10 +575,60 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>gggg</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>hggh</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">joo				</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bewolktt</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>192.168.000.000</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>255.255.255.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>du hast einen problem</t>
         </is>
       </c>
-      <c r="E1" t="n">
+      <c r="E3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -705,7 +780,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
změny na trimazkonu, import nové verze 3.7 ip_manager do trimazkonu
</commit_message>
<xml_diff>
--- a/IP_setting/saved_addresses_2.xlsx
+++ b/IP_setting/saved_addresses_2.xlsx
@@ -658,59 +658,59 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>514-2</t>
+          <t>518</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>T</t>
+          <t>V</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>\\192.168.14.245\Data\Kamery</t>
+          <t>\\192.168.208.200\10_vision</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Vision</t>
+          <t>jhv_vision</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>*Jhv2708</t>
+          <t>Jhv*2708</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>první sít, ixon</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>518</t>
+          <t>514-2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>V</t>
+          <t>T</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>\\192.168.208.200\10_vision</t>
+          <t>\\192.168.14.245\Data\Kamery</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>jhv_vision</t>
+          <t>Vision</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Jhv*2708</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>první sít, ixon</t>
+          <t>*Jhv2708</t>
         </is>
       </c>
     </row>
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>